<commit_message>
Release ver 1.0, fix location of company
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -150,7 +150,7 @@
     <t xml:space="preserve">Note: </t>
   </si>
   <si>
-    <t>31 Kênh Tiêu 1, Ấp Tiến Lân, Xã Bà Điểm, Huyện Hóc Môn, Tp.HCM</t>
+    <t>31 Kênh Tiêu 1, Ấp Tiền Lân, Xã Bà Điểm, Huyện Hóc Môn, Tp.HCM</t>
   </si>
 </sst>
 </file>
@@ -531,6 +531,15 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -557,15 +566,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -902,7 +902,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:G10"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,9 +922,9 @@
       <c r="G1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="41"/>
     </row>
     <row r="2" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
@@ -936,9 +936,9 @@
       <c r="G2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
@@ -950,25 +950,25 @@
       <c r="G3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="40"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
@@ -983,17 +983,17 @@
       <c r="J5" s="16"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="43"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="8"/>
       <c r="I6" s="28" t="s">
         <v>24</v>
@@ -1001,17 +1001,17 @@
       <c r="J6" s="16"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="43"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="8"/>
       <c r="I7" s="28" t="s">
         <v>28</v>
@@ -1019,17 +1019,17 @@
       <c r="J7" s="16"/>
     </row>
     <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="43"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="8"/>
       <c r="I8" s="28" t="s">
         <v>25</v>
@@ -1037,19 +1037,19 @@
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="43"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="17"/>
       <c r="D9" s="28" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="43"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="8"/>
       <c r="I9" s="28" t="s">
         <v>26</v>
@@ -1057,19 +1057,19 @@
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="43"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="8"/>
       <c r="D10" s="28" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="43"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="8"/>
       <c r="I10" s="28" t="s">
         <v>27</v>
@@ -1077,19 +1077,19 @@
       <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="43"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="17"/>
       <c r="D11" s="28" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="43"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="8"/>
       <c r="I11" s="28" t="s">
         <v>30</v>
@@ -1097,19 +1097,19 @@
       <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="43"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="8"/>
       <c r="D12" s="28" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="43" t="s">
+      <c r="F12" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="43"/>
+      <c r="G12" s="34"/>
       <c r="H12" s="8"/>
       <c r="I12" s="28" t="s">
         <v>31</v>
@@ -1129,7 +1129,7 @@
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:10" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1161,7 +1161,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
@@ -1708,6 +1708,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J1:J3"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F6:G6"/>
@@ -1724,14 +1732,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J1:J3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
18/06/24 - Changed logo image
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -589,15 +589,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>33617</xdr:colOff>
+      <xdr:colOff>51287</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>44824</xdr:rowOff>
+      <xdr:rowOff>34768</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>857250</xdr:colOff>
+      <xdr:colOff>805962</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>226575</xdr:rowOff>
+      <xdr:rowOff>278422</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -620,8 +620,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33617" y="44824"/>
-          <a:ext cx="5386108" cy="705626"/>
+          <a:off x="51287" y="34768"/>
+          <a:ext cx="4996963" cy="851789"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -901,8 +901,8 @@
   </sheetPr>
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,7 +912,7 @@
     <col min="3" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10"/>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -926,7 +926,7 @@
       <c r="I1" s="40"/>
       <c r="J1" s="41"/>
     </row>
-    <row r="2" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -940,7 +940,7 @@
       <c r="I2" s="40"/>
       <c r="J2" s="42"/>
     </row>
-    <row r="3" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1734,7 +1734,7 @@
     <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="77" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="76" orientation="portrait" r:id="rId1"/>
   <headerFooter differentOddEven="1" differentFirst="1">
     <oddHeader>&amp;L&amp;G&amp;R&amp;"Arial,nghiêng đậm"&amp;16BÁO CÁO KIỂM TRA BƠM</oddHeader>
     <firstHeader>&amp;R&amp;"Arial,đậm"&amp;18BÁO CÁO KIỂM TRA BƠM</firstHeader>

</xml_diff>